<commit_message>
updating automatic YAML creation script
</commit_message>
<xml_diff>
--- a/Camera_pos.xlsx
+++ b/Camera_pos.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -394,42 +394,22 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>-43.19058609008789</v>
+        <v>133.2647857666016</v>
       </c>
       <c r="B2">
-        <v>-10.95882320404053</v>
+        <v>164.2115020751953</v>
       </c>
       <c r="C2">
-        <v>0.6572868227958679</v>
+        <v>25.46099853515625</v>
       </c>
       <c r="D2">
-        <v>5.193960078031523E-06</v>
+        <v>1.402960788254859E-05</v>
       </c>
       <c r="E2">
-        <v>2.416145086288452</v>
+        <v>-31.57320404052734</v>
       </c>
       <c r="F2">
-        <v>-171.1515655517578</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3">
-        <v>-70.30057525634766</v>
-      </c>
-      <c r="B3">
-        <v>22.72959136962891</v>
-      </c>
-      <c r="C3">
-        <v>2.694149732589722</v>
-      </c>
-      <c r="D3">
-        <v>4.616170826921007E-06</v>
-      </c>
-      <c r="E3">
-        <v>0.8062422871589661</v>
-      </c>
-      <c r="F3">
-        <v>-91.43100738525391</v>
+        <v>89.66863250732422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>